<commit_message>
Do tests for the logic
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail/Romain Lenoir/Journal_de_travail_I_Shoes.xlsx
+++ b/Documentation/Journal_de_travail/Romain Lenoir/Journal_de_travail_I_Shoes.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sacha.JACCARD\Documents\GitHub\I_Shoes\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romai\Romain\GitHub DATA\I_Shoes\Documentation\Journal_de_travail\Romain Lenoir\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D56EB71-517A-4C16-8466-7C0EF737C3E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7680" yWindow="1200" windowWidth="15510" windowHeight="11295"/>
+    <workbookView xWindow="7680" yWindow="1200" windowWidth="15510" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal_de_travail" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
   <si>
     <t>Date</t>
   </si>
@@ -68,9 +69,6 @@
     <t>Sacha</t>
   </si>
   <si>
-    <t>Alex</t>
-  </si>
-  <si>
     <t>Login</t>
   </si>
   <si>
@@ -97,11 +95,17 @@
   <si>
     <t>Création de la page d'accueil, une navbar est présente avec le nom de l'utilisateur connecter et le bouton logout ou login si l'utilisateur est déconnecté</t>
   </si>
+  <si>
+    <t>Erreur</t>
+  </si>
+  <si>
+    <t>Corrige certaines erreurs et fait des tests afin de rendre le code et le site plus fluide</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="hh:mm:ss;@"/>
   </numFmts>
@@ -237,16 +241,6 @@
   <dxfs count="6">
     <dxf>
       <font>
-        <color theme="7"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -276,6 +270,16 @@
     <dxf>
       <numFmt numFmtId="164" formatCode="hh:mm:ss;@"/>
     </dxf>
+    <dxf>
+      <font>
+        <color theme="7"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -290,22 +294,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:H1007" totalsRowShown="0">
-  <autoFilter ref="A1:H1007"/>
-  <sortState ref="A2:H3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="A1:H1007" totalsRowShown="0">
+  <autoFilter ref="A1:H1007" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H3">
     <sortCondition ref="A1:A6"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" name="Date"/>
-    <tableColumn id="2" name="Début" dataDxfId="5"/>
-    <tableColumn id="3" name="Fin" dataDxfId="4"/>
-    <tableColumn id="4" name="Durée" dataDxfId="3">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Début" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Fin" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Durée" dataDxfId="1">
       <calculatedColumnFormula>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Thème"/>
-    <tableColumn id="6" name="Nom de présence"/>
-    <tableColumn id="7" name="Description"/>
-    <tableColumn id="8" name="Sources" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Thème"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Nom de présence"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Description"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Sources" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -573,11 +577,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1103"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J1101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -650,13 +654,13 @@
         <v>8.333333333333337E-2</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>7</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H3" s="10"/>
     </row>
@@ -675,13 +679,13 @@
         <v>1.041666666666663E-2</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>7</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H4" s="11"/>
     </row>
@@ -700,13 +704,13 @@
         <v>2.083333333333337E-2</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>7</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H5" s="16"/>
     </row>
@@ -725,13 +729,13 @@
         <v>1.736111111111116E-2</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>7</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H6" s="11"/>
     </row>
@@ -750,13 +754,13 @@
         <v>3.4722222222222321E-2</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>7</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H7" s="12"/>
     </row>
@@ -775,13 +779,13 @@
         <v>0.25</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>7</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H8" s="11"/>
     </row>
@@ -800,27 +804,39 @@
         <v>8.333333333333337E-2</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>7</v>
       </c>
       <c r="G9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" s="11"/>
+    </row>
+    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>44962</v>
+      </c>
+      <c r="B10" s="8">
+        <v>0.55902777777777779</v>
+      </c>
+      <c r="C10" s="8">
+        <v>0.59375</v>
+      </c>
+      <c r="D10" s="9">
+        <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
+        <v>3.472222222222221E-2</v>
+      </c>
+      <c r="E10" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="11"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="9">
-        <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
-        <v>0</v>
-      </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
+      <c r="F10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>21</v>
+      </c>
       <c r="H10" s="12"/>
       <c r="I10" s="3"/>
     </row>
@@ -8522,30 +8538,20 @@
         <v>7</v>
       </c>
     </row>
-    <row r="1102" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1102" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="1103" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1103" t="s">
-        <v>11</v>
-      </c>
-    </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="timePeriod" dxfId="1" priority="1" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="5" priority="1" timePeriod="today">
       <formula>FLOOR(A1,1)=TODAY()</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="0" priority="2" timePeriod="yesterday">
+    <cfRule type="timePeriod" dxfId="4" priority="2" timePeriod="yesterday">
       <formula>FLOOR(A1,1)=TODAY()-1</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$A$1101:$A$1103</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1099">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1099" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>$A$1101:$A$1102</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Journal de travail de Sacha à jour
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail/Romain Lenoir/Journal_de_travail_I_Shoes.xlsx
+++ b/Documentation/Journal_de_travail/Romain Lenoir/Journal_de_travail_I_Shoes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sacha.JACCARD\Documents\GitHub\I_Shoes\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sacha.JACCARD\Documents\GitHub\I_Shoes\Documentation\Journal_de_travail\Romain Lenoir\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
   <si>
     <t>Date</t>
   </si>
@@ -105,7 +105,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="hh:mm:ss;@"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,12 +156,6 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="8"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -184,7 +178,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -223,11 +217,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -290,8 +279,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:H1007" totalsRowShown="0">
-  <autoFilter ref="A1:H1007"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:H1006" totalsRowShown="0">
+  <autoFilter ref="A1:H1006"/>
   <sortState ref="A2:H3">
     <sortCondition ref="A1:A6"/>
   </sortState>
@@ -574,10 +563,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1103"/>
+  <dimension ref="A1:J1102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,38 +605,44 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="18">
+    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
         <v>44959</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="5">
         <v>0.5625</v>
       </c>
-      <c r="C2" s="1">
-        <v>0.62152777777777779</v>
-      </c>
-      <c r="D2" s="17">
-        <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
-        <v>5.902777777777779E-2</v>
-      </c>
-      <c r="F2" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="14"/>
-    </row>
-    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+      <c r="C2" s="8">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="D2" s="9">
+        <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="10"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
         <v>44959</v>
       </c>
-      <c r="B3" s="5">
-        <v>0.5625</v>
+      <c r="B3" s="8">
+        <v>0.65625</v>
       </c>
       <c r="C3" s="8">
-        <v>0.64583333333333337</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="D3" s="9">
         <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
-        <v>8.333333333333337E-2</v>
+        <v>1.041666666666663E-2</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>12</v>
@@ -656,23 +651,23 @@
         <v>7</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="10"/>
+        <v>14</v>
+      </c>
+      <c r="H3" s="11"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>44959</v>
       </c>
       <c r="B4" s="8">
-        <v>0.65625</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="C4" s="8">
-        <v>0.66666666666666663</v>
+        <v>0.6875</v>
       </c>
       <c r="D4" s="9">
         <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
-        <v>1.041666666666663E-2</v>
+        <v>2.083333333333337E-2</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>12</v>
@@ -681,23 +676,23 @@
         <v>7</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="11"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="H4" s="16"/>
+    </row>
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>44959</v>
       </c>
       <c r="B5" s="8">
-        <v>0.66666666666666663</v>
+        <v>0.6875</v>
       </c>
       <c r="C5" s="8">
-        <v>0.6875</v>
+        <v>0.70486111111111116</v>
       </c>
       <c r="D5" s="9">
         <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
-        <v>2.083333333333337E-2</v>
+        <v>1.736111111111116E-2</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>12</v>
@@ -706,23 +701,23 @@
         <v>7</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" s="16"/>
-    </row>
-    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="H5" s="11"/>
+    </row>
+    <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
-        <v>44959</v>
+        <v>44961</v>
       </c>
       <c r="B6" s="8">
-        <v>0.6875</v>
+        <v>0.67013888888888884</v>
       </c>
       <c r="C6" s="8">
         <v>0.70486111111111116</v>
       </c>
       <c r="D6" s="9">
         <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
-        <v>1.736111111111116E-2</v>
+        <v>3.4722222222222321E-2</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>12</v>
@@ -731,23 +726,23 @@
         <v>7</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" s="11"/>
-    </row>
-    <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="H6" s="12"/>
+    </row>
+    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>44961</v>
       </c>
       <c r="B7" s="8">
-        <v>0.67013888888888884</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="C7" s="8">
-        <v>0.70486111111111116</v>
+        <v>0.95833333333333337</v>
       </c>
       <c r="D7" s="9">
         <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
-        <v>3.4722222222222321E-2</v>
+        <v>0.25</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>12</v>
@@ -756,59 +751,48 @@
         <v>7</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" s="12"/>
-    </row>
-    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="H7" s="11"/>
+    </row>
+    <row r="8" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
-        <v>44961</v>
+        <v>44962</v>
       </c>
       <c r="B8" s="8">
-        <v>0.70833333333333337</v>
+        <v>0.34027777777777773</v>
       </c>
       <c r="C8" s="8">
-        <v>0.95833333333333337</v>
+        <v>0.4236111111111111</v>
       </c>
       <c r="D8" s="9">
         <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
-        <v>0.25</v>
+        <v>8.333333333333337E-2</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>7</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H8" s="11"/>
     </row>
-    <row r="9" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
-        <v>44962</v>
-      </c>
-      <c r="B9" s="8">
-        <v>0.34027777777777773</v>
-      </c>
-      <c r="C9" s="8">
-        <v>0.4236111111111111</v>
-      </c>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="7"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
       <c r="D9" s="9">
         <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
-        <v>8.333333333333337E-2</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="H9" s="11"/>
+        <v>0</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="3"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
@@ -821,8 +805,8 @@
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="3"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="6"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
@@ -836,7 +820,6 @@
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="11"/>
-      <c r="I11" s="6"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
@@ -888,7 +871,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
-      <c r="H15" s="11"/>
+      <c r="H15" s="13"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
@@ -940,7 +923,9 @@
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="13"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
@@ -968,9 +953,7 @@
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
+      <c r="H21" s="13"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
@@ -1048,7 +1031,7 @@
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
-      <c r="H27" s="13"/>
+      <c r="H27" s="12"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
@@ -1061,7 +1044,7 @@
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
-      <c r="H28" s="12"/>
+      <c r="H28" s="13"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
@@ -1191,7 +1174,7 @@
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="13"/>
+      <c r="H38" s="11"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
@@ -1204,7 +1187,8 @@
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="11"/>
+      <c r="H39" s="12"/>
+      <c r="I39" s="13"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
@@ -1217,8 +1201,7 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="12"/>
-      <c r="I40" s="13"/>
+      <c r="H40" s="6"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
@@ -1231,7 +1214,7 @@
       <c r="E41" s="6"/>
       <c r="F41" s="6"/>
       <c r="G41" s="6"/>
-      <c r="H41" s="6"/>
+      <c r="H41" s="11"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
@@ -1245,6 +1228,7 @@
       <c r="F42" s="6"/>
       <c r="G42" s="6"/>
       <c r="H42" s="11"/>
+      <c r="I42" s="6"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="7"/>
@@ -1257,8 +1241,8 @@
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="11"/>
-      <c r="I43" s="6"/>
+      <c r="H43" s="12"/>
+      <c r="I43" s="13"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="7"/>
@@ -1271,8 +1255,7 @@
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="12"/>
-      <c r="I44" s="13"/>
+      <c r="H44" s="11"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
@@ -1285,7 +1268,7 @@
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="11"/>
+      <c r="H45" s="13"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="7"/>
@@ -1298,7 +1281,7 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="13"/>
+      <c r="H46" s="11"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="7"/>
@@ -1311,7 +1294,7 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="11"/>
+      <c r="H47" s="12"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="7"/>
@@ -1324,7 +1307,7 @@
       <c r="E48" s="6"/>
       <c r="F48" s="6"/>
       <c r="G48" s="6"/>
-      <c r="H48" s="12"/>
+      <c r="H48" s="13"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="7"/>
@@ -1350,7 +1333,8 @@
       <c r="E50" s="6"/>
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
-      <c r="H50" s="13"/>
+      <c r="H50" s="12"/>
+      <c r="I50" s="11"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="7"/>
@@ -1363,8 +1347,7 @@
       <c r="E51" s="6"/>
       <c r="F51" s="6"/>
       <c r="G51" s="6"/>
-      <c r="H51" s="12"/>
-      <c r="I51" s="11"/>
+      <c r="H51" s="13"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="7"/>
@@ -1403,7 +1386,8 @@
       <c r="E54" s="6"/>
       <c r="F54" s="6"/>
       <c r="G54" s="6"/>
-      <c r="H54" s="13"/>
+      <c r="H54" s="12"/>
+      <c r="I54" s="11"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="7"/>
@@ -1416,8 +1400,7 @@
       <c r="E55" s="6"/>
       <c r="F55" s="6"/>
       <c r="G55" s="6"/>
-      <c r="H55" s="12"/>
-      <c r="I55" s="11"/>
+      <c r="H55" s="14"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="7"/>
@@ -1469,7 +1452,8 @@
       <c r="E59" s="6"/>
       <c r="F59" s="6"/>
       <c r="G59" s="6"/>
-      <c r="H59" s="14"/>
+      <c r="H59" s="12"/>
+      <c r="I59" s="6"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="7"/>
@@ -1482,8 +1466,7 @@
       <c r="E60" s="6"/>
       <c r="F60" s="6"/>
       <c r="G60" s="6"/>
-      <c r="H60" s="12"/>
-      <c r="I60" s="6"/>
+      <c r="H60" s="14"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="7"/>
@@ -1522,7 +1505,7 @@
       <c r="E63" s="6"/>
       <c r="F63" s="6"/>
       <c r="G63" s="6"/>
-      <c r="H63" s="14"/>
+      <c r="H63" s="12"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="7"/>
@@ -1535,7 +1518,7 @@
       <c r="E64" s="6"/>
       <c r="F64" s="6"/>
       <c r="G64" s="6"/>
-      <c r="H64" s="12"/>
+      <c r="H64" s="11"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="7"/>
@@ -1548,7 +1531,7 @@
       <c r="E65" s="6"/>
       <c r="F65" s="6"/>
       <c r="G65" s="6"/>
-      <c r="H65" s="11"/>
+      <c r="H65" s="12"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="7"/>
@@ -1561,7 +1544,7 @@
       <c r="E66" s="6"/>
       <c r="F66" s="6"/>
       <c r="G66" s="6"/>
-      <c r="H66" s="12"/>
+      <c r="H66" s="11"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="7"/>
@@ -1574,7 +1557,7 @@
       <c r="E67" s="6"/>
       <c r="F67" s="6"/>
       <c r="G67" s="6"/>
-      <c r="H67" s="11"/>
+      <c r="H67" s="15"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="7"/>
@@ -1600,7 +1583,7 @@
       <c r="E69" s="6"/>
       <c r="F69" s="6"/>
       <c r="G69" s="6"/>
-      <c r="H69" s="15"/>
+      <c r="H69" s="14"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="7"/>
@@ -1616,16 +1599,10 @@
       <c r="H70" s="14"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" s="7"/>
-      <c r="B71" s="8"/>
-      <c r="C71" s="8"/>
       <c r="D71" s="9">
         <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
         <v>0</v>
       </c>
-      <c r="E71" s="6"/>
-      <c r="F71" s="6"/>
-      <c r="G71" s="6"/>
       <c r="H71" s="14"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
@@ -8174,11 +8151,8 @@
       <c r="H1006" s="14"/>
     </row>
     <row r="1007" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D1007" s="9">
-        <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
-        <v>0</v>
-      </c>
-      <c r="H1007" s="14"/>
+      <c r="D1007" s="2"/>
+      <c r="H1007" s="3"/>
     </row>
     <row r="1008" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D1008" s="2"/>
@@ -8401,7 +8375,6 @@
       <c r="H1062" s="3"/>
     </row>
     <row r="1063" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D1063" s="2"/>
       <c r="H1063" s="3"/>
     </row>
     <row r="1064" spans="4:8" x14ac:dyDescent="0.25">
@@ -8510,25 +8483,22 @@
       <c r="H1098" s="3"/>
     </row>
     <row r="1099" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H1099" s="3"/>
+      <c r="A1099" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="1100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1100" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="1101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1101" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="1102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1102" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="1103" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1103" t="s">
         <v>11</v>
       </c>
     </row>
@@ -8542,11 +8512,11 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F1048576">
-      <formula1>$A$1101:$A$1103</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576">
+      <formula1>$A$1100:$A$1102</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1099">
-      <formula1>$A$1101:$A$1102</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1098">
+      <formula1>$A$1100:$A$1101</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Work on the acceuil page
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail/Romain Lenoir/Journal_de_travail_I_Shoes.xlsx
+++ b/Documentation/Journal_de_travail/Romain Lenoir/Journal_de_travail_I_Shoes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romai\Romain\GitHub DATA\I_Shoes\Documentation\Journal_de_travail\Romain Lenoir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B122C2-185A-44C2-A012-62B6C6EBC4C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AC9A46E-E566-4540-AE97-734C44F6F9B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7680" yWindow="1200" windowWidth="15510" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8025" yWindow="1545" windowWidth="15510" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal_de_travail" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
   <si>
     <t>Date</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>Crée une variable de session pour le logge de l'admin et optimise le code</t>
+  </si>
+  <si>
+    <t>Crée l'interface principal de la page d'acceuil.</t>
   </si>
 </sst>
 </file>
@@ -586,8 +589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J1101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -872,17 +875,29 @@
       <c r="H11" s="11"/>
       <c r="I11" s="6"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
+    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>44977</v>
+      </c>
+      <c r="B12" s="8">
+        <v>0.33680555555555558</v>
+      </c>
+      <c r="C12" s="8">
+        <v>0.36805555555555558</v>
+      </c>
       <c r="D12" s="9">
         <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
-        <v>0</v>
-      </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="H12" s="11"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Create Carousel, not with bootstrap
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail/Romain Lenoir/Journal_de_travail_I_Shoes.xlsx
+++ b/Documentation/Journal_de_travail/Romain Lenoir/Journal_de_travail_I_Shoes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romai\Romain\GitHub DATA\I_Shoes\Documentation\Journal_de_travail\Romain Lenoir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5719D52A-DFE6-463F-90B0-824847714929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9691F6E8-6037-4634-9037-73273DB5FB7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8025" yWindow="1545" windowWidth="15510" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="29">
   <si>
     <t>Date</t>
   </si>
@@ -115,6 +115,12 @@
   </si>
   <si>
     <t>Alex Barreira-Videira</t>
+  </si>
+  <si>
+    <t>Crée et configure un carousel contemplatif pour les différentes chaussures</t>
+  </si>
+  <si>
+    <t>M. MEYLAN</t>
   </si>
 </sst>
 </file>
@@ -605,8 +611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J1101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -930,18 +936,32 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
+    <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
+        <v>44985</v>
+      </c>
+      <c r="B14" s="8">
+        <v>0.67013888888888884</v>
+      </c>
+      <c r="C14" s="8">
+        <v>0.70138888888888884</v>
+      </c>
       <c r="D14" s="9">
         <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
-        <v>0</v>
-      </c>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="11"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H14" s="20" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>

</xml_diff>

<commit_message>
Optimize the code, do stocks in cases and in json file and admin stuff
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail/Romain Lenoir/Journal_de_travail_I_Shoes.xlsx
+++ b/Documentation/Journal_de_travail/Romain Lenoir/Journal_de_travail_I_Shoes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romai\Romain\GitHub DATA\I_Shoes\Documentation\Journal_de_travail\Romain Lenoir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2BC25EE-DB89-4C51-9DFC-ACAE9BF4E174}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{741475AD-0670-47CF-A2C4-F9C024921812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8025" yWindow="1545" windowWidth="15510" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -142,6 +142,15 @@
   </si>
   <si>
     <t>Modifie le contenu de toutes les pages selon la méthodologie des articles, change un peu de mise en page pour les cases d'articles</t>
+  </si>
+  <si>
+    <t>Variables de sessions et articles</t>
+  </si>
+  <si>
+    <t>Renchéris la base de données des articles en fichier json et gère les stocks. Optimise les cases et s'ocupent de toutes les pages</t>
+  </si>
+  <si>
+    <t>Termine de gérer correctement les stocks et optimise une nouvelle fois les cases</t>
   </si>
 </sst>
 </file>
@@ -632,8 +641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J1101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1084,30 +1093,54 @@
       </c>
       <c r="H18" s="13"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
+    <row r="19" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="7">
+        <v>44991</v>
+      </c>
+      <c r="B19" s="8">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="C19" s="8">
+        <v>0.81597222222222221</v>
+      </c>
       <c r="D19" s="9">
         <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
-        <v>0</v>
-      </c>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
+        <v>8.680555555555558E-2</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="H19" s="13"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
+    <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="7">
+        <v>44991</v>
+      </c>
+      <c r="B20" s="8">
+        <v>0.88541666666666663</v>
+      </c>
+      <c r="C20" s="8">
+        <v>0.90277777777777779</v>
+      </c>
       <c r="D20" s="9">
         <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
-        <v>0</v>
-      </c>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
+        <v>1.736111111111116E-2</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="H20" s="11"/>
       <c r="I20" s="6"/>
       <c r="J20" s="6"/>

</xml_diff>

<commit_message>
Update the work diary
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail/Romain Lenoir/Journal_de_travail_I_Shoes.xlsx
+++ b/Documentation/Journal_de_travail/Romain Lenoir/Journal_de_travail_I_Shoes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romai\Romain\GitHub DATA\I_Shoes\Documentation\Journal_de_travail\Romain Lenoir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F69D3E6-F964-4C80-A2C5-282B2EF612A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B2AD2A-747A-4495-AD5C-30EB1E440494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8025" yWindow="1545" windowWidth="15510" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="58">
   <si>
     <t>Date</t>
   </si>
@@ -203,6 +203,12 @@
   <si>
     <t>https://www.w3schools.com/php/func_array_splice.asp</t>
   </si>
+  <si>
+    <t>JSON data and more</t>
+  </si>
+  <si>
+    <t>Crée une nouvelle page liéeà la récapitulatif d'articles et optimise le code pour faire cet effet</t>
+  </si>
 </sst>
 </file>
 
@@ -305,7 +311,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -355,6 +361,9 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -703,8 +712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J1101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1440,18 +1449,32 @@
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="7"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
+    <row r="30" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="7">
+        <v>45007</v>
+      </c>
+      <c r="B30" s="8">
+        <v>0.59722222222222221</v>
+      </c>
+      <c r="C30" s="8">
+        <v>0.72361111111111109</v>
+      </c>
       <c r="D30" s="9">
         <f>SUM(Tableau1[[#This Row],[Fin]]-Tableau1[[#This Row],[Début]])</f>
-        <v>0</v>
-      </c>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="13"/>
+        <v>0.12638888888888888</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="H30" s="22" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>

</xml_diff>